<commit_message>
Documentation - Correction des erreurs
</commit_message>
<xml_diff>
--- a/Documentation/05 UseCases - Scenarii/useCases-Scenarii.xlsx
+++ b/Documentation/05 UseCases - Scenarii/useCases-Scenarii.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WebAppGestionRepas\Documentation\05 UseCases - Scenarii\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CE0CA2-729E-407C-B993-9640EF2B76FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC10F4D0-857B-4A41-9E34-EE2658EEDC56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="817" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="817" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Use-case_Visiteur" sheetId="1" r:id="rId1"/>
@@ -176,9 +176,6 @@
     <t>C</t>
   </si>
   <si>
-    <t>Acceder à la page d'accueil</t>
-  </si>
-  <si>
     <t>Avoir un aperçu de la plateforme</t>
   </si>
   <si>
@@ -191,9 +188,6 @@
     <t>M</t>
   </si>
   <si>
-    <t>Avoir des fonctionalités suplémentaire en fonction du type d'utilisateur</t>
-  </si>
-  <si>
     <t>Je clique sur le bouton [profil]</t>
   </si>
   <si>
@@ -212,9 +206,6 @@
     <t>Je clique sur [Me connecter]</t>
   </si>
   <si>
-    <t>le user ou le mdp est incorrect</t>
-  </si>
-  <si>
     <t>Le compte est de type Administrateur</t>
   </si>
   <si>
@@ -257,30 +248,12 @@
     <t>Affiche un message pour informer qu'un compte existe déjà</t>
   </si>
   <si>
-    <t>le mail n'est pas un type mail valide</t>
-  </si>
-  <si>
     <t>Affiche un message pour informer que le mail est incorrect</t>
   </si>
   <si>
-    <t>La confirmation et le mdp ne sont pas similaire</t>
-  </si>
-  <si>
     <t>Affiche un message pour informer que le mdp n'est pas 2 fois le même</t>
   </si>
   <si>
-    <t>Les critères du mdp ne sont pas réspecter</t>
-  </si>
-  <si>
-    <t>Affiche un message pour informer quel critères sont demandé</t>
-  </si>
-  <si>
-    <t>Les champs obligatoire ne sont pas tous ramplis</t>
-  </si>
-  <si>
-    <t>Affiche un message pour informer qu'il manque des information</t>
-  </si>
-  <si>
     <t>Tout est correct</t>
   </si>
   <si>
@@ -320,9 +293,6 @@
     <t>Modifier un menu</t>
   </si>
   <si>
-    <t>Personaliser un menu avec les plats souhaité</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
@@ -332,15 +302,9 @@
     <t>Je clique sur [Ajouter un menu]</t>
   </si>
   <si>
-    <t>Je choisi un nom pour le menu</t>
-  </si>
-  <si>
     <t>Je clique sur [Valider le menu]</t>
   </si>
   <si>
-    <t>une popup s'affiche avec un champ pour le nom du menu</t>
-  </si>
-  <si>
     <t>Le champ "Nom du menu" est vide</t>
   </si>
   <si>
@@ -359,18 +323,9 @@
     <t>Affichage de la page "Ajout d'un plat"</t>
   </si>
   <si>
-    <t>Je choisi un plat dans la liste</t>
-  </si>
-  <si>
-    <t>Je choisi le nombre de personnes</t>
-  </si>
-  <si>
     <t>Je clique sur [Ajouter le plat au menu]</t>
   </si>
   <si>
-    <t>Aucun plat n'est séléctionné</t>
-  </si>
-  <si>
     <t>Une erreur s'affiche "Un plat est obligatoire"</t>
   </si>
   <si>
@@ -413,18 +368,9 @@
     <t>Affiche la liste des propositions "Une enseigne" et "Toutes les enseignes"</t>
   </si>
   <si>
-    <t>Je choisi "Toute les enseignes"</t>
-  </si>
-  <si>
     <t>Affichage de la liste des ingrédients les moins cher peu importe l'enseigne</t>
   </si>
   <si>
-    <t>Je choisi "Une les enseigne"</t>
-  </si>
-  <si>
-    <t>Affichage de la liste des ingrédients pour l'enseigne la moin cher</t>
-  </si>
-  <si>
     <t>Me déconnecter</t>
   </si>
   <si>
@@ -443,9 +389,6 @@
     <t>Administrateur</t>
   </si>
   <si>
-    <t>gérer les utilisateurs</t>
-  </si>
-  <si>
     <t>Ajouter ou modifier un utilisateur</t>
   </si>
   <si>
@@ -470,9 +413,6 @@
     <t>Les conditions pour le "register" sont remplis</t>
   </si>
   <si>
-    <t>Affiche la page des utilisateur avec l'utilisateur modifié</t>
-  </si>
-  <si>
     <t>Je clique sur [Supprimer l'utilisateur]</t>
   </si>
   <si>
@@ -485,9 +425,6 @@
     <t>Je clique sur [Valider la modification]</t>
   </si>
   <si>
-    <t>Affiche la page des utilisateur avec l'utilisateur créé</t>
-  </si>
-  <si>
     <t>Affiche un message de confirmation "Êtes vous sûr de vouloir supprimer l'utilisateur …"</t>
   </si>
   <si>
@@ -497,12 +434,6 @@
     <t>Affiche la page des utilisateur sans l'utilisateur supprimé</t>
   </si>
   <si>
-    <t>gérer les recettes</t>
-  </si>
-  <si>
-    <t>Proposer une liste de recettes variée</t>
-  </si>
-  <si>
     <t>Je clique sur la page "Recettes"</t>
   </si>
   <si>
@@ -536,9 +467,6 @@
     <t>Affiche l'erreur "La recettes doit avoir des ingrédients"</t>
   </si>
   <si>
-    <t>Tout est remplis</t>
-  </si>
-  <si>
     <t>Affiche la page "Recettes" avec la recette ajoutée</t>
   </si>
   <si>
@@ -554,9 +482,6 @@
     <t>Affiche la page "Recettes" sans la recette supprimée"</t>
   </si>
   <si>
-    <t>gérer les articles</t>
-  </si>
-  <si>
     <t>Proposer une liste d'articles disponibles dans plusieurs enseignes</t>
   </si>
   <si>
@@ -584,9 +509,6 @@
     <t>Affiche l'erreur "L'article doit avoir un prix"</t>
   </si>
   <si>
-    <t>L'enseinge n'est pas séléctionnée</t>
-  </si>
-  <si>
     <t>Affiche l'erreur "Une enseigne doit être séléctionnée"</t>
   </si>
   <si>
@@ -614,9 +536,6 @@
     <t>Affiche un message de confirmation "Êtes vous sûr de vouloir supprimer l'article …"</t>
   </si>
   <si>
-    <t>Affiche la page "Articles" sans l'article supprimée"</t>
-  </si>
-  <si>
     <t>10 - Ajouter et modifier un article</t>
   </si>
   <si>
@@ -645,6 +564,87 @@
   </si>
   <si>
     <t>01 - Afficher la page d'accueil</t>
+  </si>
+  <si>
+    <t>Accéder à la page d'accueil</t>
+  </si>
+  <si>
+    <t>l'utilisateur ou le mot de passe est incorrect</t>
+  </si>
+  <si>
+    <t>Avoir des fonctionalités suplémentaires en fonction du type d'utilisateur</t>
+  </si>
+  <si>
+    <t>Le mail n'est pas un type mail valide</t>
+  </si>
+  <si>
+    <t>La confirmation et le mdp ne sont pas similaires</t>
+  </si>
+  <si>
+    <t>Les critères du mdp ne sont pas respectés</t>
+  </si>
+  <si>
+    <t>Les champs obligatoires ne sont pas tous remplis</t>
+  </si>
+  <si>
+    <t>Affiche un message pour informer quel critères sont demandés</t>
+  </si>
+  <si>
+    <t>Affiche un message pour informer qu'il manque des informations</t>
+  </si>
+  <si>
+    <t>Je choisis un nom pour le menu</t>
+  </si>
+  <si>
+    <t>Je choisis un plat dans la liste</t>
+  </si>
+  <si>
+    <t>Je choisis le nombre de personnes</t>
+  </si>
+  <si>
+    <t>Aucun plat n'est sélectionné</t>
+  </si>
+  <si>
+    <t>Un pop-up s'affiche avec un champ pour le nom du menu</t>
+  </si>
+  <si>
+    <t>Personnaliser un menu avec les plats souhaités</t>
+  </si>
+  <si>
+    <t>Je choisis "Toute les enseignes"</t>
+  </si>
+  <si>
+    <t>Je choisis "Une les enseigne"</t>
+  </si>
+  <si>
+    <t>Affichage de la liste des ingrédients pour l'enseigne la moin chère</t>
+  </si>
+  <si>
+    <t>Gérer les utilisateurs</t>
+  </si>
+  <si>
+    <t>Affiche la page des utilisateurs avec l'utilisateur créé</t>
+  </si>
+  <si>
+    <t>Affiche la page des utilisateurs avec l'utilisateur modifié</t>
+  </si>
+  <si>
+    <t>Proposer une liste de recettes variées</t>
+  </si>
+  <si>
+    <t>Tout est rempli</t>
+  </si>
+  <si>
+    <t>Gérer les articles</t>
+  </si>
+  <si>
+    <t>Gérer les recettes</t>
+  </si>
+  <si>
+    <t>L'enseigne n'est pas sélectionnée</t>
+  </si>
+  <si>
+    <t>Affiche la page "Articles" sans l'article supprimé</t>
   </si>
 </sst>
 </file>
@@ -2385,7 +2385,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>générer une liste de commissions</a:t>
+            <a:t>Générer une liste de commissions</a:t>
           </a:r>
           <a:endParaRPr lang="fr-CH">
             <a:effectLst/>
@@ -3509,7 +3509,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>163</v>
+        <v>136</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -3520,7 +3520,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -3531,7 +3531,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
@@ -3542,7 +3542,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>5</v>
@@ -3553,7 +3553,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3571,26 +3571,26 @@
     <row r="9" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="26"/>
       <c r="C9" s="19" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="D9" s="20"/>
     </row>
     <row r="10" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="10" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="27" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -3606,7 +3606,9 @@
   </sheetPr>
   <dimension ref="B1:D16"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3627,7 +3629,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -3638,7 +3640,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -3649,7 +3651,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>102</v>
+        <v>161</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
@@ -3660,7 +3662,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>5</v>
@@ -3671,7 +3673,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3689,75 +3691,75 @@
     <row r="9" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="26"/>
       <c r="C9" s="19" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="D9" s="20"/>
     </row>
     <row r="10" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="10" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="10" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>116</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="23" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="10" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="23" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>110</v>
+        <v>91</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>111</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="23" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="10" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="27" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="12" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -3773,7 +3775,9 @@
   </sheetPr>
   <dimension ref="B1:D18"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3794,7 +3798,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -3805,7 +3809,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -3816,7 +3820,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>120</v>
+        <v>167</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
@@ -3827,7 +3831,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>121</v>
+        <v>164</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>5</v>
@@ -3838,7 +3842,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3856,93 +3860,93 @@
     <row r="9" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="26"/>
       <c r="C9" s="19" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="D9" s="20"/>
     </row>
     <row r="10" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="10" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="10" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="33" t="s">
-        <v>125</v>
+        <v>102</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="34"/>
       <c r="C13" s="9" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="32"/>
       <c r="C14" s="9" t="s">
-        <v>133</v>
+        <v>165</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>134</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="23" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="10" t="s">
-        <v>153</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="23" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="23" t="s">
-        <v>127</v>
+        <v>104</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="10" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="27" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="12" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -3961,7 +3965,9 @@
   </sheetPr>
   <dimension ref="B1:D19"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3982,7 +3988,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>160</v>
+        <v>133</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -3993,7 +3999,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -4004,7 +4010,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
@@ -4015,7 +4021,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>140</v>
+        <v>115</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>5</v>
@@ -4026,7 +4032,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4044,102 +4050,102 @@
     <row r="9" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="26"/>
       <c r="C9" s="19" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="D9" s="20"/>
     </row>
     <row r="10" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="10" t="s">
-        <v>123</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>142</v>
+        <v>117</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="10" t="s">
-        <v>143</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="33" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>145</v>
+        <v>120</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>146</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="34"/>
       <c r="C13" s="9" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="34"/>
       <c r="C14" s="9" t="s">
-        <v>149</v>
+        <v>168</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="32"/>
       <c r="C15" s="9" t="s">
-        <v>133</v>
+        <v>165</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="23" t="s">
-        <v>152</v>
+        <v>126</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="10" t="s">
-        <v>154</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="23" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>155</v>
+        <v>129</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>156</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="23" t="s">
-        <v>157</v>
+        <v>131</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="10" t="s">
-        <v>158</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="27" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="12" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -4169,7 +4175,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF87318-A59A-4DEC-8F43-37E7476413E6}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -4186,7 +4192,9 @@
   </sheetPr>
   <dimension ref="B1:D16"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4207,7 +4215,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>169</v>
+        <v>142</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -4218,7 +4226,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -4229,7 +4237,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>13</v>
+        <v>143</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
@@ -4240,7 +4248,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>5</v>
@@ -4268,11 +4276,11 @@
     </row>
     <row r="9" spans="2:4" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="18" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -4294,7 +4302,9 @@
   </sheetPr>
   <dimension ref="B1:D17"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4315,7 +4325,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>168</v>
+        <v>141</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -4326,7 +4336,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -4337,7 +4347,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
@@ -4348,7 +4358,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>18</v>
+        <v>145</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>5</v>
@@ -4359,7 +4369,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4376,58 +4386,58 @@
     </row>
     <row r="9" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="31" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="32"/>
       <c r="C10" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="10"/>
     </row>
     <row r="12" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="33" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>25</v>
+        <v>144</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="34"/>
       <c r="C13" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="35"/>
       <c r="C14" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -4453,7 +4463,9 @@
   </sheetPr>
   <dimension ref="B1:D17"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4474,7 +4486,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -4485,7 +4497,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -4496,7 +4508,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
@@ -4507,7 +4519,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>18</v>
+        <v>145</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>5</v>
@@ -4518,7 +4530,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4536,80 +4548,80 @@
     <row r="9" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="22"/>
       <c r="C9" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D9" s="10"/>
     </row>
     <row r="10" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="21" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="10"/>
     </row>
     <row r="12" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="33" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="34"/>
       <c r="C13" s="9" t="s">
-        <v>40</v>
+        <v>146</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="34"/>
       <c r="C14" s="9" t="s">
-        <v>42</v>
+        <v>147</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="34"/>
       <c r="C15" s="9" t="s">
-        <v>44</v>
+        <v>148</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>45</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="34"/>
       <c r="C16" s="24" t="s">
-        <v>46</v>
+        <v>149</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>47</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="2:4" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="35"/>
       <c r="C17" s="11" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -4649,7 +4661,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>166</v>
+        <v>139</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -4660,7 +4672,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -4671,7 +4683,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
@@ -4682,7 +4694,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>5</v>
@@ -4711,35 +4723,35 @@
     <row r="9" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="26"/>
       <c r="C9" s="19" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D9" s="20"/>
     </row>
     <row r="10" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="10" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="10" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="27" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C12" s="11"/>
       <c r="D12" s="12" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -4755,7 +4767,9 @@
   </sheetPr>
   <dimension ref="B1:D21"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4776,7 +4790,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>165</v>
+        <v>138</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -4787,7 +4801,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -4798,7 +4812,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
@@ -4809,7 +4823,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>61</v>
+        <v>157</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>5</v>
@@ -4820,7 +4834,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -4838,114 +4852,114 @@
     <row r="9" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="26"/>
       <c r="C9" s="19" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D9" s="20"/>
     </row>
     <row r="10" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="10" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="10" t="s">
-        <v>67</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
-        <v>65</v>
+        <v>152</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="10"/>
     </row>
     <row r="13" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="36" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="36"/>
       <c r="C14" s="9" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="23" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="10" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="23" t="s">
-        <v>74</v>
+        <v>153</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="10"/>
     </row>
     <row r="17" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="23" t="s">
-        <v>75</v>
+        <v>154</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="10"/>
     </row>
     <row r="18" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="33" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>77</v>
+        <v>155</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="32"/>
       <c r="C19" s="9" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="23" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="10" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="27" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="12" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -4965,7 +4979,9 @@
   </sheetPr>
   <dimension ref="B1:D14"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4986,7 +5002,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>164</v>
+        <v>137</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -4997,7 +5013,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>7</v>
@@ -5008,7 +5024,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
@@ -5019,7 +5035,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>61</v>
+        <v>157</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>5</v>
@@ -5030,7 +5046,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5048,53 +5064,53 @@
     <row r="9" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="26"/>
       <c r="C9" s="19" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D9" s="20"/>
     </row>
     <row r="10" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="10" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="23" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="10" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="23" t="s">
-        <v>92</v>
+        <v>158</v>
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="10" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="23" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="10" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="27" t="s">
-        <v>94</v>
+        <v>159</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="12" t="s">
-        <v>95</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>